<commit_message>
update the design document.
</commit_message>
<xml_diff>
--- a/doc/ladderConnectionMap.xlsx
+++ b/doc/ladderConnectionMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Works\NCL\Project\Metro_emulator\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A50BF4-88FD-49A0-B657-E18933EFC8D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50D3BFA-9081-4565-8FFF-6062656D9BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="149">
   <si>
     <t>we-s0</t>
   </si>
@@ -477,6 +477,12 @@
   </si>
   <si>
     <t>PLC07[regs addresses]</t>
+  </si>
+  <si>
+    <t>Station Sensors ID</t>
+  </si>
+  <si>
+    <t>Q1.0</t>
   </si>
 </sst>
 </file>
@@ -846,7 +852,7 @@
   <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P32" sqref="P32"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,7 +890,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="3" t="s">
-        <v>78</v>
+        <v>147</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>84</v>
@@ -1335,7 +1341,7 @@
         <v>83</v>
       </c>
       <c r="S10" t="s">
-        <v>54</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1382,7 +1388,7 @@
         <v>83</v>
       </c>
       <c r="S11" t="s">
-        <v>55</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update the design document and added the readme of the realworld simulator's readme file.
</commit_message>
<xml_diff>
--- a/doc/ladderConnectionMap.xlsx
+++ b/doc/ladderConnectionMap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Works\NCL\Project\Metro_emulator\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50D3BFA-9081-4565-8FFF-6062656D9BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB33233-B5DC-46FE-AD72-C72613DFF26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5265" yWindow="1500" windowWidth="29100" windowHeight="13230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="151">
   <si>
     <t>we-s0</t>
   </si>
@@ -483,6 +483,12 @@
   </si>
   <si>
     <t>Q1.0</t>
+  </si>
+  <si>
+    <t>PLC07 [regs addresses]</t>
+  </si>
+  <si>
+    <t>no ladder logic</t>
   </si>
 </sst>
 </file>
@@ -849,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:V40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,12 +875,13 @@
     <col min="12" max="12" width="13.28515625" customWidth="1"/>
     <col min="13" max="13" width="14.140625" customWidth="1"/>
     <col min="14" max="14" width="11.85546875" customWidth="1"/>
-    <col min="17" max="17" width="12.28515625" customWidth="1"/>
-    <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" customWidth="1"/>
+    <col min="17" max="19" width="12.28515625" customWidth="1"/>
+    <col min="20" max="20" width="16.140625" customWidth="1"/>
+    <col min="21" max="21" width="14" customWidth="1"/>
+    <col min="22" max="22" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>78</v>
       </c>
@@ -918,10 +925,17 @@
         <v>145</v>
       </c>
       <c r="S1" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="V1" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -962,13 +976,22 @@
         <v>134</v>
       </c>
       <c r="R2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="T2" t="s">
+        <v>150</v>
+      </c>
+      <c r="U2" t="s">
         <v>111</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V2" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1009,13 +1032,22 @@
         <v>135</v>
       </c>
       <c r="R3" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="T3" t="s">
+        <v>150</v>
+      </c>
+      <c r="U3" t="s">
         <v>112</v>
       </c>
-      <c r="S3" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V3" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1056,13 +1088,22 @@
         <v>136</v>
       </c>
       <c r="R4" t="s">
+        <v>41</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="T4" t="s">
+        <v>150</v>
+      </c>
+      <c r="U4" t="s">
         <v>113</v>
       </c>
-      <c r="S4" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V4" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1103,13 +1144,22 @@
         <v>137</v>
       </c>
       <c r="R5" t="s">
+        <v>42</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="T5" t="s">
+        <v>150</v>
+      </c>
+      <c r="U5" t="s">
         <v>114</v>
       </c>
-      <c r="S5" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V5" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1150,13 +1200,22 @@
         <v>139</v>
       </c>
       <c r="R6" t="s">
+        <v>43</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="T6" t="s">
+        <v>150</v>
+      </c>
+      <c r="U6" t="s">
         <v>115</v>
       </c>
-      <c r="S6" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V6" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1197,13 +1256,22 @@
         <v>140</v>
       </c>
       <c r="R7" t="s">
+        <v>44</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="T7" t="s">
+        <v>150</v>
+      </c>
+      <c r="U7" t="s">
         <v>116</v>
       </c>
-      <c r="S7" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V7" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1244,13 +1312,22 @@
         <v>141</v>
       </c>
       <c r="R8" t="s">
+        <v>45</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="T8" t="s">
+        <v>150</v>
+      </c>
+      <c r="U8" t="s">
         <v>117</v>
       </c>
-      <c r="S8" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V8" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1291,13 +1368,22 @@
         <v>142</v>
       </c>
       <c r="R9" t="s">
+        <v>46</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="T9" t="s">
+        <v>150</v>
+      </c>
+      <c r="U9" t="s">
         <v>118</v>
       </c>
-      <c r="S9" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V9" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1341,10 +1427,19 @@
         <v>83</v>
       </c>
       <c r="S10" t="s">
+        <v>39</v>
+      </c>
+      <c r="T10" t="s">
+        <v>150</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="V10" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1388,10 +1483,19 @@
         <v>83</v>
       </c>
       <c r="S11" t="s">
+        <v>40</v>
+      </c>
+      <c r="T11" t="s">
+        <v>150</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="V11" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1428,9 +1532,9 @@
       <c r="N12" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="R12" s="2"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U12" s="2"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1467,9 +1571,9 @@
       <c r="N13" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="R13" s="2"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U13" s="2"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1506,9 +1610,9 @@
       <c r="N14" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="R14" s="2"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U14" s="2"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1545,9 +1649,9 @@
       <c r="N15" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="R15" s="2"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U15" s="2"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1584,9 +1688,9 @@
       <c r="N16" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="R16" s="2"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="U16" s="2"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1623,9 +1727,9 @@
       <c r="N17" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="R17" s="2"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="U17" s="2"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1663,7 +1767,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1701,7 +1805,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1739,7 +1843,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1777,7 +1881,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1815,7 +1919,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -1853,7 +1957,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1868,7 +1972,7 @@
       </c>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1882,7 +1986,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -1897,7 +2001,7 @@
       </c>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -1912,7 +2016,7 @@
       </c>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1926,7 +2030,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1940,7 +2044,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -1954,7 +2058,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -1968,7 +2072,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>21</v>
       </c>

</xml_diff>